<commit_message>
Edits to the dash board
Joined trafficking data into one graph.
Joined cropraids data into one graph.
Added icons to the arrests table.
Removed the fill effect from the key.
species trend graph.
Changed the colors to one graphical color for each animal.
</commit_message>
<xml_diff>
--- a/GVTC/keyspecies.xlsx
+++ b/GVTC/keyspecies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GVTC\startbootstrap-sb-admin-gh-pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evet\Documents\GitHub\GVTC_Webmaps\GVTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A113456-66CE-4270-959B-E1A1F1F3F71C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6422942-B891-4671-90EE-1BF90F86D8E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{55F120E2-28E6-427E-B449-91B098924D2E}"/>
   </bookViews>
@@ -35,10 +35,10 @@
     <t>Hippos</t>
   </si>
   <si>
-    <t>Golliras</t>
+    <t>Elephants</t>
   </si>
   <si>
-    <t>Elephants</t>
+    <t>Gorillas</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>8000</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>13000</v>

</xml_diff>

<commit_message>
modify all the pages
</commit_message>
<xml_diff>
--- a/GVTC/keyspecies.xlsx
+++ b/GVTC/keyspecies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evet\Documents\GitHub\GVTC_Webmaps\GVTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GVTC\startbootstrap-sb-admin-gh-pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6422942-B891-4671-90EE-1BF90F86D8E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A113456-66CE-4270-959B-E1A1F1F3F71C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{55F120E2-28E6-427E-B449-91B098924D2E}"/>
   </bookViews>
@@ -35,10 +35,10 @@
     <t>Hippos</t>
   </si>
   <si>
-    <t>Elephants</t>
+    <t>Golliras</t>
   </si>
   <si>
-    <t>Gorillas</t>
+    <t>Elephants</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>8000</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>13000</v>

</xml_diff>